<commit_message>
Datos ventas cerdo 2021
</commit_message>
<xml_diff>
--- a/GV/RegistroInformacion.xlsx
+++ b/GV/RegistroInformacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natasha GO\Desktop\Granja\Granja\GV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920F3F2-0BA2-43F9-A3A9-A55FAE6A9E1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E2B35-1D07-4977-BDEE-E419CB380665}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294792477" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="158">
   <si>
     <t>CERDOS</t>
   </si>
@@ -596,10 +596,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -917,7 +918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -958,13 +959,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -973,23 +985,17 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -998,7 +1004,7 @@
   <dxfs count="108">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1008,41 +1014,328 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1056,131 +1349,16 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1282,6 +1460,192 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -2701,364 +3065,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3890,67 +3896,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB0CB5FE-EC69-4A3C-B7F8-2A2B829875A7}" name="VentaCerdo" displayName="VentaCerdo" ref="A3:M122" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
-  <autoFilter ref="A3:M122" xr:uid="{C9EBBED2-E078-4EE1-9F48-7C43C603BD9F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB0CB5FE-EC69-4A3C-B7F8-2A2B829875A7}" name="VentaCerdo" displayName="VentaCerdo" ref="A3:M139" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A3:M139" xr:uid="{C9EBBED2-E078-4EE1-9F48-7C43C603BD9F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:M122">
     <sortCondition ref="D3:D122"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AF79EB7F-53B6-458F-84BF-82950CA97A22}" name="Año" dataDxfId="105">
+    <tableColumn id="1" xr3:uid="{AF79EB7F-53B6-458F-84BF-82950CA97A22}" name="Año" dataDxfId="12">
       <calculatedColumnFormula>YEAR(VentaCerdo[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{19A051CF-8C1B-4292-8170-4118C1548088}" name="Mes" dataDxfId="104">
+    <tableColumn id="32" xr3:uid="{19A051CF-8C1B-4292-8170-4118C1548088}" name="Mes" dataDxfId="11">
       <calculatedColumnFormula>MONTH(VentaCerdo[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{6C2E3871-F892-4AAA-80F8-BCBBAF515294}" name="Semana" dataDxfId="103">
+    <tableColumn id="30" xr3:uid="{6C2E3871-F892-4AAA-80F8-BCBBAF515294}" name="Semana" dataDxfId="10">
       <calculatedColumnFormula>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{B8618162-D69B-4A8A-8D93-DA3328E46CB0}" name="FECHA" dataDxfId="102"/>
-    <tableColumn id="27" xr3:uid="{C9E3266E-0727-428C-9BF1-A7AD09AE9EAF}" name="Almacen" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{08C0B01F-B3AD-4119-8859-A6491FD939BC}" name="Kilos Salidas" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{404682AC-60FB-4D7E-B817-BD2248526A86}" name="Kilos Cancelados" dataDxfId="99"/>
-    <tableColumn id="4" xr3:uid="{69CCC8E0-14F6-464A-8ECF-15DB81E956CA}" name="Cabezas Salidas" dataDxfId="98"/>
-    <tableColumn id="5" xr3:uid="{582FE33C-0D80-475D-BE61-AFEF1986FB0B}" name="Cabezas Entradas" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{5DC4E71E-F9FC-4F43-96C9-2941B4DB0D05}" name="Importe Ventas" dataDxfId="96" dataCellStyle="Moneda"/>
-    <tableColumn id="7" xr3:uid="{789D5740-B7CD-4B88-BD7F-0439A78EE71F}" name="Importe Costos" dataDxfId="95" dataCellStyle="Moneda"/>
-    <tableColumn id="8" xr3:uid="{21DA54D1-A1D1-476A-AAFA-CCA51CAAD970}" name="No. Ventas" dataDxfId="94" dataCellStyle="Moneda"/>
-    <tableColumn id="9" xr3:uid="{5F292483-6A0F-4601-BDA1-69CB1520DF6A}" name="No. Cancelaciones" dataDxfId="93" dataCellStyle="Moneda"/>
+    <tableColumn id="29" xr3:uid="{B8618162-D69B-4A8A-8D93-DA3328E46CB0}" name="FECHA" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{C9E3266E-0727-428C-9BF1-A7AD09AE9EAF}" name="Almacen" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{08C0B01F-B3AD-4119-8859-A6491FD939BC}" name="Kilos Salidas" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{404682AC-60FB-4D7E-B817-BD2248526A86}" name="Kilos Cancelados" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{69CCC8E0-14F6-464A-8ECF-15DB81E956CA}" name="Cabezas Salidas" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{582FE33C-0D80-475D-BE61-AFEF1986FB0B}" name="Cabezas Entradas" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{5DC4E71E-F9FC-4F43-96C9-2941B4DB0D05}" name="Importe Ventas" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="7" xr3:uid="{789D5740-B7CD-4B88-BD7F-0439A78EE71F}" name="Importe Costos" dataDxfId="2" dataCellStyle="Moneda"/>
+    <tableColumn id="8" xr3:uid="{21DA54D1-A1D1-476A-AAFA-CCA51CAAD970}" name="No. Ventas" dataDxfId="1" dataCellStyle="Moneda"/>
+    <tableColumn id="9" xr3:uid="{5F292483-6A0F-4601-BDA1-69CB1520DF6A}" name="No. Cancelaciones" dataDxfId="0" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF896AA2-B65B-4FCE-818D-A2F40213676F}" name="VentaBorrego" displayName="VentaBorrego" ref="A3:N42" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF896AA2-B65B-4FCE-818D-A2F40213676F}" name="VentaBorrego" displayName="VentaBorrego" ref="A3:N42" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A3:N42" xr:uid="{38DBC52E-8295-4265-BD99-782A589694BE}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{BD5E6769-D0E8-4F54-880B-5D38062AAF9A}" name="Año" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{BD5E6769-D0E8-4F54-880B-5D38062AAF9A}" name="Año" dataDxfId="65">
       <calculatedColumnFormula>YEAR(VentaBorrego[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{14A4283D-6080-4AEE-9DFB-7811E2F62E2B}" name="Mes" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{14A4283D-6080-4AEE-9DFB-7811E2F62E2B}" name="Mes" dataDxfId="64">
       <calculatedColumnFormula>MONTH(VentaBorrego[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{82A091B3-D16B-4CE7-AA3D-FA4F05EDA4BA}" name="Semana" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{82A091B3-D16B-4CE7-AA3D-FA4F05EDA4BA}" name="Semana" dataDxfId="63">
       <calculatedColumnFormula>WEEKNUM(VentaBorrego[[#This Row],[FECHA]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{13F5AFB3-77AC-44D0-961F-823E68D126F3}" name="FECHA" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{EBDDF3F9-0C0A-4094-AA1F-B2D397AB66A1}" name="PZA / CABEZA" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{1D78316A-F810-4621-B59B-6F206C31ECCE}" name="Granja" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{E000B50B-F6FB-4F0F-BD43-C09E32FC0162}" name="Kilos Total" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{D1555C53-BD42-42F2-929D-D387FAF35155}" name="Kilos Cancelados" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{F3438513-7B19-4D28-AB39-40BCE1C169BE}" name="Cabezas Salidas" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{897F88A8-933A-486C-AF8B-B272BBA93476}" name="Cabezas Entradas" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{434ABA26-D192-4815-8FC2-8380C56F30E1}" name="Importe Ventas" dataDxfId="40"/>
-    <tableColumn id="12" xr3:uid="{5360CB49-C259-428D-A326-744802978D19}" name="Importe Costos" dataDxfId="39"/>
-    <tableColumn id="13" xr3:uid="{45F67444-6C73-4B85-96D1-DE35910222FD}" name="No. Ventas" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{8238E6F8-EF54-4793-BA99-0035F6738AFB}" name="No. Cancelaciones" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{13F5AFB3-77AC-44D0-961F-823E68D126F3}" name="FECHA" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{EBDDF3F9-0C0A-4094-AA1F-B2D397AB66A1}" name="PZA / CABEZA" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{1D78316A-F810-4621-B59B-6F206C31ECCE}" name="Granja" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{E000B50B-F6FB-4F0F-BD43-C09E32FC0162}" name="Kilos Total" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{D1555C53-BD42-42F2-929D-D387FAF35155}" name="Kilos Cancelados" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{F3438513-7B19-4D28-AB39-40BCE1C169BE}" name="Cabezas Salidas" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{897F88A8-933A-486C-AF8B-B272BBA93476}" name="Cabezas Entradas" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{434ABA26-D192-4815-8FC2-8380C56F30E1}" name="Importe Ventas" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{5360CB49-C259-428D-A326-744802978D19}" name="Importe Costos" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{45F67444-6C73-4B85-96D1-DE35910222FD}" name="No. Ventas" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{8238E6F8-EF54-4793-BA99-0035F6738AFB}" name="No. Cancelaciones" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{8651429E-3CCF-4283-963F-CE1D86878DE3}" name="NB" displayName="NB" ref="P3:V4" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{8651429E-3CCF-4283-963F-CE1D86878DE3}" name="NB" displayName="NB" ref="P3:V4" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="P3:V4" xr:uid="{F3E1A5D4-2206-4A5B-8082-DCC730185F04}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F593C191-662A-4A08-9C07-3BC417717AF5}" name="AÑO">
@@ -3962,17 +3968,17 @@
     <tableColumn id="3" xr3:uid="{AC94EA02-7DE1-43F2-9333-779EF3503D3B}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(NB[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{262F6740-57C6-42B0-95B2-CA81288CD2CD}" name="Fecha" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{86F88214-2BD2-441F-8F5D-6918680F83CC}" name="Producto" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{CB17BC44-E2BE-4CCE-AAD8-2D70C83B4842}" name="Almacén" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{20B296C9-926F-4D06-B340-1B3183A1F0E5}" name="Entrada" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{262F6740-57C6-42B0-95B2-CA81288CD2CD}" name="Fecha" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{86F88214-2BD2-441F-8F5D-6918680F83CC}" name="Producto" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{CB17BC44-E2BE-4CCE-AAD8-2D70C83B4842}" name="Almacén" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{20B296C9-926F-4D06-B340-1B3183A1F0E5}" name="Entrada" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{87BC9115-FF64-4CCD-870C-F5486EBE0BF6}" name="MB" displayName="MB" ref="X3:AD4" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{87BC9115-FF64-4CCD-870C-F5486EBE0BF6}" name="MB" displayName="MB" ref="X3:AD4" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="X3:AD4" xr:uid="{C07E5018-4C77-46A8-A50B-107FA9C88156}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1E8E5BF2-508C-417D-BE57-3AACF0C714C5}" name="AÑO">
@@ -3984,10 +3990,10 @@
     <tableColumn id="3" xr3:uid="{0BD97616-9EFF-4FF6-9E9B-D9B72CED3912}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(MB[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7F573887-B59C-4BEE-9E01-7A8C9A0FB227}" name="Fecha" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{C91C4368-6E38-4907-8554-722F18CCA7AC}" name="Descripción" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{8E66D7C9-E4E6-43F9-B89C-603982C07332}" name="Almacén" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{77D0FF8F-7647-48FF-A88B-9E8A6485B51B}" name="Salida" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{7F573887-B59C-4BEE-9E01-7A8C9A0FB227}" name="Fecha" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{C91C4368-6E38-4907-8554-722F18CCA7AC}" name="Descripción" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{8E66D7C9-E4E6-43F9-B89C-603982C07332}" name="Almacén" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{77D0FF8F-7647-48FF-A88B-9E8A6485B51B}" name="Salida" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4004,10 +4010,10 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{87D3F1B1-9BFB-4962-B1E1-B5A3B607B8E6}" name="PNC" displayName="PNC" ref="C1:C6" totalsRowShown="0" dataDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{87D3F1B1-9BFB-4962-B1E1-B5A3B607B8E6}" name="PNC" displayName="PNC" ref="C1:C6" totalsRowShown="0" dataDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="C1:C6" xr:uid="{79BD6A38-95D5-48F5-B30F-01B067AA4A61}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E272FD8D-EB97-4C4A-B51C-B3A7AF0EBA0A}" name="ProductoNacimiento" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{E272FD8D-EB97-4C4A-B51C-B3A7AF0EBA0A}" name="ProductoNacimiento" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4064,7 +4070,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7FA5903A-793D-41AF-927E-0E5AEF940163}" name="NC" displayName="NC" ref="O3:U4" totalsRowShown="0" headerRowDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7FA5903A-793D-41AF-927E-0E5AEF940163}" name="NC" displayName="NC" ref="O3:U4" totalsRowShown="0" headerRowDxfId="107">
   <autoFilter ref="O3:U4" xr:uid="{02D5D0CD-EDA4-456A-A5E8-9F3730BDF858}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C0348CA9-B923-4DF2-B7B8-6F0BEEF03B4F}" name="AÑO">
@@ -4076,10 +4082,10 @@
     <tableColumn id="3" xr3:uid="{A92A8AB5-1C79-4CA4-B109-A49731842416}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(NC[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1E2C6755-7899-4C5E-8849-9F4DEA103FB6}" name="Fecha" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{3E44B0DD-62A3-4C63-B2ED-8D9F754BC1C8}" name="Descripción" dataDxfId="90"/>
-    <tableColumn id="7" xr3:uid="{9FD31AF2-F6BB-40A9-A5EF-A7BE8C1EE096}" name="Almacén" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{D483493A-6942-4223-8114-7C47B876A768}" name="Entrada" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{1E2C6755-7899-4C5E-8849-9F4DEA103FB6}" name="Fecha" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{3E44B0DD-62A3-4C63-B2ED-8D9F754BC1C8}" name="Descripción" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{9FD31AF2-F6BB-40A9-A5EF-A7BE8C1EE096}" name="Almacén" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{D483493A-6942-4223-8114-7C47B876A768}" name="Entrada" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4106,10 +4112,10 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FF45D115-374A-40C0-8D86-25AE41DDE243}" name="RH" displayName="RH" ref="C1:C8" totalsRowShown="0" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FF45D115-374A-40C0-8D86-25AE41DDE243}" name="RH" displayName="RH" ref="C1:C8" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="C1:C8" xr:uid="{750FC6F7-70F6-4B4E-96D7-A30F50A00065}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0F2F3A8E-A423-4F30-80DD-B0FF8E6F61FE}" name="Bodega Postura H" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{0F2F3A8E-A423-4F30-80DD-B0FF8E6F61FE}" name="Bodega Postura H" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4156,27 +4162,27 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B4177F0-5950-447A-8A7E-EECFDE618E9D}" name="DFH" displayName="DFH" ref="M1:M25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{6B4177F0-5950-447A-8A7E-EECFDE618E9D}" name="DFH" displayName="DFH" ref="M1:M25" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="M1:M25" xr:uid="{066AC525-C68B-40D3-AE6B-D275A0A79615}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{799DDA5E-B376-41AA-A689-3A660979943E}" name="Descripción" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{799DDA5E-B376-41AA-A689-3A660979943E}" name="Descripción" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{F4AC4A7A-6B8E-4F6D-84F1-88848C4BFC53}" name="AFH" displayName="AFH" ref="O1:O8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{F4AC4A7A-6B8E-4F6D-84F1-88848C4BFC53}" name="AFH" displayName="AFH" ref="O1:O8" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="O1:O8" xr:uid="{5D329DB3-7365-4EEF-8F0E-32C5AD338BA4}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A972FACD-4BAA-4284-A344-B0B89AAEF5A6}" name="Almacén" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{A972FACD-4BAA-4284-A344-B0B89AAEF5A6}" name="Almacén" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{DF3123BF-C6EE-4852-BE92-1F3C04FDF032}" name="UFH" displayName="UFH" ref="Q1:Q4" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{DF3123BF-C6EE-4852-BE92-1F3C04FDF032}" name="UFH" displayName="UFH" ref="Q1:Q4" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="Q1:Q4" xr:uid="{B76C3F68-F66F-46E8-9784-B4AAADE438F9}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7AF09891-3B17-4F67-912C-FAE5416AB3EF}" name="Unidad"/>
@@ -4186,7 +4192,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1EEBF04B-5CA7-4B0A-ADFE-2A6A9768B634}" name="MC" displayName="MC" ref="W3:AC4" totalsRowShown="0" headerRowDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1EEBF04B-5CA7-4B0A-ADFE-2A6A9768B634}" name="MC" displayName="MC" ref="W3:AC4" totalsRowShown="0" headerRowDxfId="102">
   <autoFilter ref="W3:AC4" xr:uid="{15203CCB-6A72-4C9E-82BA-A853B5165F17}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{99A49235-A43E-4B45-948E-613A29DBA5A6}" name="AÑO">
@@ -4198,10 +4204,10 @@
     <tableColumn id="3" xr3:uid="{CC8DCD94-2C62-421E-8A0B-4EE9F9AA0BA6}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(MC[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{057B6A06-06EB-4370-9C7D-67B564AB477C}" name="Fecha" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{F7D1F4AC-D899-4963-BC58-63184492E881}" name="Descripción" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{C424C129-BB09-45C4-8A52-C928098DD204}" name="Almacén" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{D7883101-3244-4BC1-AC2D-3BFB937551E5}" name="Salida" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{057B6A06-06EB-4370-9C7D-67B564AB477C}" name="Fecha" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{F7D1F4AC-D899-4963-BC58-63184492E881}" name="Descripción" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{C424C129-BB09-45C4-8A52-C928098DD204}" name="Almacén" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{D7883101-3244-4BC1-AC2D-3BFB937551E5}" name="Salida" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4292,33 +4298,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CCB7B361-D7AD-453D-B08D-6A7BDC433A61}" name="VentaHuevo" displayName="VentaHuevo" ref="A3:K106" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CCB7B361-D7AD-453D-B08D-6A7BDC433A61}" name="VentaHuevo" displayName="VentaHuevo" ref="A3:K106" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A3:K106" xr:uid="{D4382671-7652-40D0-940C-E955EF481B0A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FD9F0EF0-AAEC-44EF-B652-AEE3A7B1514D}" name="Año" dataDxfId="80">
+    <tableColumn id="1" xr3:uid="{FD9F0EF0-AAEC-44EF-B652-AEE3A7B1514D}" name="Año" dataDxfId="95">
       <calculatedColumnFormula>YEAR(VentaHuevo[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{38DF3F1A-ECDF-4B36-9176-FD4C2215E738}" name="Mes" dataDxfId="79">
+    <tableColumn id="2" xr3:uid="{38DF3F1A-ECDF-4B36-9176-FD4C2215E738}" name="Mes" dataDxfId="94">
       <calculatedColumnFormula>MONTH(VentaHuevo[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0806F8F4-F211-461B-8637-91E4CE806C4D}" name="Semana" dataDxfId="78">
+    <tableColumn id="3" xr3:uid="{0806F8F4-F211-461B-8637-91E4CE806C4D}" name="Semana" dataDxfId="93">
       <calculatedColumnFormula>WEEKNUM(VentaHuevo[[#This Row],[FECHA]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8434CCCE-DE27-4AE6-A002-E0E6CF045C72}" name="FECHA" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{779AD8B5-3C79-434E-A399-2FBAD1799E8D}" name="Postura" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{A97041C1-DD4A-498F-8E13-F603ABE564D9}" name="Kilos Total" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{CC975B41-EAF3-4B15-B675-8C8CEAE44165}" name="Kilos Cancelados" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{AC4B10C7-0849-4C4C-9BA5-AE8FB92493E2}" name="Importe Ventas" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{B2B64C19-21ED-42F7-B0F5-7AE2560707DB}" name="Importe Costos" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{777D0A0A-820D-4722-8450-983DB543ED2D}" name="No. Ventas" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{7E467BF3-DE83-4056-B631-B9B5060F190D}" name="No. Cancelaciones" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{8434CCCE-DE27-4AE6-A002-E0E6CF045C72}" name="FECHA" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{779AD8B5-3C79-434E-A399-2FBAD1799E8D}" name="Postura" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{A97041C1-DD4A-498F-8E13-F603ABE564D9}" name="Kilos Total" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{CC975B41-EAF3-4B15-B675-8C8CEAE44165}" name="Kilos Cancelados" dataDxfId="89"/>
+    <tableColumn id="8" xr3:uid="{AC4B10C7-0849-4C4C-9BA5-AE8FB92493E2}" name="Importe Ventas" dataDxfId="88"/>
+    <tableColumn id="9" xr3:uid="{B2B64C19-21ED-42F7-B0F5-7AE2560707DB}" name="Importe Costos" dataDxfId="87"/>
+    <tableColumn id="10" xr3:uid="{777D0A0A-820D-4722-8450-983DB543ED2D}" name="No. Ventas" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{7E467BF3-DE83-4056-B631-B9B5060F190D}" name="No. Cancelaciones" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B8C3BF5-B426-4FC9-8CCD-BD04125E8FC9}" name="RecoleccionHuevo" displayName="RecoleccionHuevo" ref="M3:T248" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B8C3BF5-B426-4FC9-8CCD-BD04125E8FC9}" name="RecoleccionHuevo" displayName="RecoleccionHuevo" ref="M3:T248" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="M3:T248" xr:uid="{60C9021B-900B-4B60-A55B-39BD4E52B0C3}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5556DBC3-8C5C-48FF-AC71-14BD1764535F}" name="Año">
@@ -4330,18 +4336,18 @@
     <tableColumn id="3" xr3:uid="{B97B1594-D27C-4255-B30B-9D3C3FCE7D1F}" name="Semana">
       <calculatedColumnFormula>WEEKNUM(RecoleccionHuevo[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F575BA58-C636-4CCE-AEC8-386F16DEDFFA}" name="Fecha" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{F575BA58-C636-4CCE-AEC8-386F16DEDFFA}" name="Fecha" dataDxfId="81"/>
     <tableColumn id="5" xr3:uid="{D6F82851-3690-4182-8BD9-4BE245CA5B59}" name="Bodega Origen"/>
-    <tableColumn id="6" xr3:uid="{F0B3184E-20DE-4D34-8B90-DB4940FA096B}" name="Cantidad" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{9D264A97-0E03-44D4-AE76-4CD1B7BAA7FD}" name="Kilos" dataDxfId="64"/>
-    <tableColumn id="9" xr3:uid="{89B76523-86A1-41BF-B81B-2D6DD4F17AEE}" name="Cajas" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{F0B3184E-20DE-4D34-8B90-DB4940FA096B}" name="Cantidad" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{9D264A97-0E03-44D4-AE76-4CD1B7BAA7FD}" name="Kilos" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{89B76523-86A1-41BF-B81B-2D6DD4F17AEE}" name="Cajas" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{49922715-EB52-4A65-91E4-0475F5534B83}" name="NH" displayName="NH" ref="V3:AB4" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{49922715-EB52-4A65-91E4-0475F5534B83}" name="NH" displayName="NH" ref="V3:AB4" totalsRowShown="0" headerRowDxfId="77">
   <autoFilter ref="V3:AB4" xr:uid="{9E909787-7729-4B69-B0D7-61A481011055}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{BB52ECF0-F2EE-4B65-A7D9-9EDA649B5891}" name="AÑO">
@@ -4353,17 +4359,17 @@
     <tableColumn id="3" xr3:uid="{40E66E16-55FD-40FD-8212-C14977333B21}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(NH[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4DAFF2EC-25FE-4925-B214-00D322A9AC67}" name="Fecha" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{5EA58C44-0B6E-4368-8DCF-6D66196470FC}" name="Descripción" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{97EB3DE5-BB67-459C-B513-658E8D859B6B}" name="Almacén" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{6E7BB089-A777-4CF9-A575-1F853606112B}" name="Entrada" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{4DAFF2EC-25FE-4925-B214-00D322A9AC67}" name="Fecha" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{5EA58C44-0B6E-4368-8DCF-6D66196470FC}" name="Descripción" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{97EB3DE5-BB67-459C-B513-658E8D859B6B}" name="Almacén" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{6E7BB089-A777-4CF9-A575-1F853606112B}" name="Entrada" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{08ECE305-8696-4B92-AAC1-994C138F8197}" name="MH" displayName="MH" ref="AD3:AJ4" totalsRowShown="0" headerRowDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{08ECE305-8696-4B92-AAC1-994C138F8197}" name="MH" displayName="MH" ref="AD3:AJ4" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="AD3:AJ4" xr:uid="{8AC8429F-5A18-4F92-8A2F-B1AB086595B2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2909D7D7-7DF1-42BB-B6A6-7E79BD333390}" name="AÑO">
@@ -4375,10 +4381,10 @@
     <tableColumn id="3" xr3:uid="{5BE7723A-8CFB-4D4C-B93F-00B4E59A0013}" name="SEMANA">
       <calculatedColumnFormula>WEEKNUM(MH[[#This Row],[Fecha]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E166EAA6-E7FA-47F4-8663-D36E75BD4551}" name="Fecha" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{1C4A59CE-B9EC-4404-AB42-D74C1B7D3FBC}" name="Descripción" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{0C49F5F7-A98C-41C3-BA35-87B49A7CD89C}" name="Almacén" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{D3993B0E-C1D3-4431-AE55-F8A1AECA4B2B}" name="Salida" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{E166EAA6-E7FA-47F4-8663-D36E75BD4551}" name="Fecha" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{1C4A59CE-B9EC-4404-AB42-D74C1B7D3FBC}" name="Descripción" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{0C49F5F7-A98C-41C3-BA35-87B49A7CD89C}" name="Almacén" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{D3993B0E-C1D3-4431-AE55-F8A1AECA4B2B}" name="Salida" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4671,15 +4677,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM122"/>
+  <dimension ref="A1:AM140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AE1:AG1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
@@ -4712,82 +4718,82 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
+      <c r="D1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="40"/>
+      <c r="AL1" s="40"/>
+      <c r="AM1" s="40"/>
     </row>
     <row r="2" spans="1:39" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
       <c r="N2" s="31"/>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="Z2" s="34" t="s">
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="Z2" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AH2" s="43" t="s">
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AH2" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
-      <c r="AL2" s="43"/>
-      <c r="AM2" s="43"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -10180,6 +10186,757 @@
       <c r="M122" s="8">
         <v>0</v>
       </c>
+    </row>
+    <row r="123" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B123" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C123" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>1</v>
+      </c>
+      <c r="D123" s="47">
+        <v>44198</v>
+      </c>
+      <c r="E123" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="49">
+        <v>530</v>
+      </c>
+      <c r="G123" s="49">
+        <v>0</v>
+      </c>
+      <c r="H123" s="49">
+        <v>5</v>
+      </c>
+      <c r="I123" s="49">
+        <v>0</v>
+      </c>
+      <c r="J123" s="50">
+        <v>19345</v>
+      </c>
+      <c r="K123" s="50">
+        <v>16367.69</v>
+      </c>
+      <c r="L123" s="50">
+        <v>1</v>
+      </c>
+      <c r="M123" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B124" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C124" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>1</v>
+      </c>
+      <c r="D124" s="47">
+        <v>44198</v>
+      </c>
+      <c r="E124" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" s="49">
+        <v>13455</v>
+      </c>
+      <c r="G124" s="49">
+        <v>0</v>
+      </c>
+      <c r="H124" s="49">
+        <v>114</v>
+      </c>
+      <c r="I124" s="49">
+        <v>0</v>
+      </c>
+      <c r="J124" s="50">
+        <v>485477.5</v>
+      </c>
+      <c r="K124" s="50">
+        <v>338133.66000000003</v>
+      </c>
+      <c r="L124" s="50">
+        <v>2</v>
+      </c>
+      <c r="M124" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B125" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C125" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>2</v>
+      </c>
+      <c r="D125" s="47">
+        <v>44200</v>
+      </c>
+      <c r="E125" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F125" s="49">
+        <v>1996.5</v>
+      </c>
+      <c r="G125" s="49">
+        <v>0</v>
+      </c>
+      <c r="H125" s="49">
+        <v>22</v>
+      </c>
+      <c r="I125" s="49">
+        <v>0</v>
+      </c>
+      <c r="J125" s="50">
+        <v>72811.25</v>
+      </c>
+      <c r="K125" s="50">
+        <v>60176.89</v>
+      </c>
+      <c r="L125" s="50">
+        <v>11</v>
+      </c>
+      <c r="M125" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B126" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C126" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>2</v>
+      </c>
+      <c r="D126" s="47">
+        <v>44200</v>
+      </c>
+      <c r="E126" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="49">
+        <v>37351.099999999991</v>
+      </c>
+      <c r="G126" s="49">
+        <v>0</v>
+      </c>
+      <c r="H126" s="49">
+        <v>338</v>
+      </c>
+      <c r="I126" s="49">
+        <v>0</v>
+      </c>
+      <c r="J126" s="50">
+        <v>1357823.1000000003</v>
+      </c>
+      <c r="K126" s="50">
+        <v>1176660.2900000005</v>
+      </c>
+      <c r="L126" s="50">
+        <v>68</v>
+      </c>
+      <c r="M126" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B127" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C127" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>2</v>
+      </c>
+      <c r="D127" s="47">
+        <v>44200</v>
+      </c>
+      <c r="E127" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F127" s="49">
+        <v>30666</v>
+      </c>
+      <c r="G127" s="49">
+        <v>0</v>
+      </c>
+      <c r="H127" s="49">
+        <v>264</v>
+      </c>
+      <c r="I127" s="49">
+        <v>0</v>
+      </c>
+      <c r="J127" s="50">
+        <v>1081406.2</v>
+      </c>
+      <c r="K127" s="50">
+        <v>751553.53</v>
+      </c>
+      <c r="L127" s="50">
+        <v>6</v>
+      </c>
+      <c r="M127" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B128" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C128" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>2</v>
+      </c>
+      <c r="D128" s="47">
+        <v>44200</v>
+      </c>
+      <c r="E128" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F128" s="49">
+        <v>1082</v>
+      </c>
+      <c r="G128" s="49">
+        <v>557</v>
+      </c>
+      <c r="H128" s="49">
+        <v>9</v>
+      </c>
+      <c r="I128" s="49">
+        <v>4</v>
+      </c>
+      <c r="J128" s="50">
+        <v>17245</v>
+      </c>
+      <c r="K128" s="50">
+        <v>16238.91</v>
+      </c>
+      <c r="L128" s="50">
+        <v>2</v>
+      </c>
+      <c r="M128" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B129" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C129" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>3</v>
+      </c>
+      <c r="D129" s="47">
+        <v>44207</v>
+      </c>
+      <c r="E129" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="49">
+        <v>2715</v>
+      </c>
+      <c r="G129" s="49">
+        <v>0</v>
+      </c>
+      <c r="H129" s="49">
+        <v>29</v>
+      </c>
+      <c r="I129" s="49">
+        <v>0</v>
+      </c>
+      <c r="J129" s="50">
+        <v>95380.5</v>
+      </c>
+      <c r="K129" s="50">
+        <v>80617.739999999991</v>
+      </c>
+      <c r="L129" s="50">
+        <v>13</v>
+      </c>
+      <c r="M129" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B130" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C130" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>3</v>
+      </c>
+      <c r="D130" s="47">
+        <v>44207</v>
+      </c>
+      <c r="E130" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="49">
+        <v>32772.399999999994</v>
+      </c>
+      <c r="G130" s="49">
+        <v>0</v>
+      </c>
+      <c r="H130" s="49">
+        <v>284</v>
+      </c>
+      <c r="I130" s="49">
+        <v>0</v>
+      </c>
+      <c r="J130" s="50">
+        <v>1160187.7000000002</v>
+      </c>
+      <c r="K130" s="50">
+        <v>995179.52000000025</v>
+      </c>
+      <c r="L130" s="50">
+        <v>68</v>
+      </c>
+      <c r="M130" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B131" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C131" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>3</v>
+      </c>
+      <c r="D131" s="47">
+        <v>44207</v>
+      </c>
+      <c r="E131" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="49">
+        <v>7435</v>
+      </c>
+      <c r="G131" s="49">
+        <v>0</v>
+      </c>
+      <c r="H131" s="49">
+        <v>63</v>
+      </c>
+      <c r="I131" s="49">
+        <v>0</v>
+      </c>
+      <c r="J131" s="50">
+        <v>260275</v>
+      </c>
+      <c r="K131" s="50">
+        <v>188658.46000000002</v>
+      </c>
+      <c r="L131" s="50">
+        <v>3</v>
+      </c>
+      <c r="M131" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B132" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C132" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>3</v>
+      </c>
+      <c r="D132" s="47">
+        <v>44207</v>
+      </c>
+      <c r="E132" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F132" s="49">
+        <v>19490</v>
+      </c>
+      <c r="G132" s="49">
+        <v>122</v>
+      </c>
+      <c r="H132" s="49">
+        <v>81</v>
+      </c>
+      <c r="I132" s="49">
+        <v>1</v>
+      </c>
+      <c r="J132" s="50">
+        <v>342972</v>
+      </c>
+      <c r="K132" s="50">
+        <v>220845.04</v>
+      </c>
+      <c r="L132" s="50">
+        <v>4</v>
+      </c>
+      <c r="M132" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B133" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C133" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>4</v>
+      </c>
+      <c r="D133" s="47">
+        <v>44214</v>
+      </c>
+      <c r="E133" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="49">
+        <v>26039.4</v>
+      </c>
+      <c r="G133" s="49">
+        <v>321.39999999999998</v>
+      </c>
+      <c r="H133" s="49">
+        <v>227</v>
+      </c>
+      <c r="I133" s="49">
+        <v>3</v>
+      </c>
+      <c r="J133" s="50">
+        <v>894312</v>
+      </c>
+      <c r="K133" s="50">
+        <v>578180.94000000018</v>
+      </c>
+      <c r="L133" s="50">
+        <v>55</v>
+      </c>
+      <c r="M133" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B134" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C134" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>4</v>
+      </c>
+      <c r="D134" s="47">
+        <v>44214</v>
+      </c>
+      <c r="E134" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="49">
+        <v>10512</v>
+      </c>
+      <c r="G134" s="49">
+        <v>10</v>
+      </c>
+      <c r="H134" s="49">
+        <v>106</v>
+      </c>
+      <c r="I134" s="49">
+        <v>10</v>
+      </c>
+      <c r="J134" s="50">
+        <v>359374.4</v>
+      </c>
+      <c r="K134" s="50">
+        <v>224933.3</v>
+      </c>
+      <c r="L134" s="50">
+        <v>4</v>
+      </c>
+      <c r="M134" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A135" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B135" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C135" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>4</v>
+      </c>
+      <c r="D135" s="47">
+        <v>44214</v>
+      </c>
+      <c r="E135" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" s="49">
+        <v>18575.12</v>
+      </c>
+      <c r="G135" s="49">
+        <v>0</v>
+      </c>
+      <c r="H135" s="49">
+        <v>116</v>
+      </c>
+      <c r="I135" s="49">
+        <v>0</v>
+      </c>
+      <c r="J135" s="50">
+        <v>445373.2</v>
+      </c>
+      <c r="K135" s="50">
+        <v>303573.81999999995</v>
+      </c>
+      <c r="L135" s="50">
+        <v>26</v>
+      </c>
+      <c r="M135" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B136" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C136" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>5</v>
+      </c>
+      <c r="D136" s="47">
+        <v>44221</v>
+      </c>
+      <c r="E136" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" s="49">
+        <v>9499</v>
+      </c>
+      <c r="G136" s="49">
+        <v>0</v>
+      </c>
+      <c r="H136" s="49">
+        <v>90</v>
+      </c>
+      <c r="I136" s="49">
+        <v>0</v>
+      </c>
+      <c r="J136" s="50">
+        <v>324966.25</v>
+      </c>
+      <c r="K136" s="50">
+        <v>247406.68999999986</v>
+      </c>
+      <c r="L136" s="50">
+        <v>28</v>
+      </c>
+      <c r="M136" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B137" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C137" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>5</v>
+      </c>
+      <c r="D137" s="47">
+        <v>44221</v>
+      </c>
+      <c r="E137" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F137" s="49">
+        <v>25285.3</v>
+      </c>
+      <c r="G137" s="49">
+        <v>804.5</v>
+      </c>
+      <c r="H137" s="49">
+        <v>227</v>
+      </c>
+      <c r="I137" s="49">
+        <v>7</v>
+      </c>
+      <c r="J137" s="50">
+        <v>835695.3</v>
+      </c>
+      <c r="K137" s="50">
+        <v>711463.20000000019</v>
+      </c>
+      <c r="L137" s="50">
+        <v>54</v>
+      </c>
+      <c r="M137" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B138" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C138" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>5</v>
+      </c>
+      <c r="D138" s="47">
+        <v>44221</v>
+      </c>
+      <c r="E138" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="49">
+        <v>23470.800000000003</v>
+      </c>
+      <c r="G138" s="49">
+        <v>0</v>
+      </c>
+      <c r="H138" s="49">
+        <v>203</v>
+      </c>
+      <c r="I138" s="49">
+        <v>0</v>
+      </c>
+      <c r="J138" s="50">
+        <v>794032.8</v>
+      </c>
+      <c r="K138" s="50">
+        <v>501381.18999999994</v>
+      </c>
+      <c r="L138" s="50">
+        <v>10</v>
+      </c>
+      <c r="M138" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A139" s="46">
+        <f>YEAR(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>2021</v>
+      </c>
+      <c r="B139" s="46">
+        <f>MONTH(VentaCerdo[[#This Row],[FECHA]])</f>
+        <v>1</v>
+      </c>
+      <c r="C139" s="46">
+        <f>WEEKNUM(VentaCerdo[[#This Row],[FECHA]],2)</f>
+        <v>5</v>
+      </c>
+      <c r="D139" s="47">
+        <v>44221</v>
+      </c>
+      <c r="E139" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" s="49">
+        <v>15125.900000000001</v>
+      </c>
+      <c r="G139" s="49">
+        <v>113.2</v>
+      </c>
+      <c r="H139" s="49">
+        <v>98</v>
+      </c>
+      <c r="I139" s="49">
+        <v>1</v>
+      </c>
+      <c r="J139" s="50">
+        <v>362398.39999999997</v>
+      </c>
+      <c r="K139" s="50">
+        <v>298935.31</v>
+      </c>
+      <c r="L139" s="50">
+        <v>12</v>
+      </c>
+      <c r="M139" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D140" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10206,7 +10963,7 @@
           <x14:formula1>
             <xm:f>ListasCerdo!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E122</xm:sqref>
+          <xm:sqref>E4:E139</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C36725EF-B06F-4509-8254-2CEC4261F233}">
           <x14:formula1>
@@ -10292,96 +11049,96 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="39"/>
-      <c r="AP1" s="39"/>
-      <c r="AQ1" s="39"/>
-      <c r="AR1" s="39"/>
-      <c r="AS1" s="39"/>
-      <c r="AT1" s="39"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
     </row>
     <row r="2" spans="1:46" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="M2" s="38" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="M2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="Y2" s="36" t="s">
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="Y2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AG2" s="34" t="s">
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AG2" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AO2" s="43" t="s">
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AO2" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="AP2" s="43"/>
-      <c r="AQ2" s="43"/>
-      <c r="AR2" s="43"/>
-      <c r="AS2" s="43"/>
-      <c r="AT2" s="43"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
     </row>
     <row r="3" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -20991,65 +21748,65 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="41"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
     </row>
     <row r="2" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="S2" s="36" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="S2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="AA2" s="34" t="s">
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="AA2" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -23065,8 +23822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051A8DC-641C-49D6-8AC0-A75FC51D70EC}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23416,13 +24173,13 @@
       <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="O1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="34" t="s">
         <v>127</v>
       </c>
     </row>
@@ -23509,7 +24266,7 @@
       <c r="O4" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="Q4" s="35" t="s">
         <v>157</v>
       </c>
     </row>
@@ -23586,7 +24343,7 @@
       <c r="M8" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="O8" s="45" t="s">
+      <c r="O8" s="35" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>